<commit_message>
homework helper scripts and GANTT chart for project
</commit_message>
<xml_diff>
--- a/Class/ECO 266 Work Breakdown.xlsx
+++ b/Class/ECO 266 Work Breakdown.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C793A0-24D7-4283-8E1A-329B06F9860B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED5FD1A-2351-4497-81DF-2A42BCA1BEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,23 +937,23 @@
     <xf numFmtId="12" fontId="5" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1621,7 +1621,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1667,186 +1667,186 @@
         <v>39</v>
       </c>
       <c r="B3" s="62"/>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="98">
+      <c r="D3" s="98"/>
+      <c r="E3" s="96">
         <v>44802</v>
       </c>
-      <c r="F3" s="98"/>
+      <c r="F3" s="96"/>
     </row>
     <row r="4" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="94"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="95">
+      <c r="I4" s="93">
         <f>I5</f>
         <v>44802</v>
       </c>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="95">
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="93">
         <f>P5</f>
         <v>44809</v>
       </c>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="96"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="96"/>
-      <c r="U4" s="96"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="95">
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
+      <c r="S4" s="94"/>
+      <c r="T4" s="94"/>
+      <c r="U4" s="94"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="93">
         <f>W5</f>
         <v>44816</v>
       </c>
-      <c r="X4" s="96"/>
-      <c r="Y4" s="96"/>
-      <c r="Z4" s="96"/>
-      <c r="AA4" s="96"/>
-      <c r="AB4" s="96"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="95">
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="95"/>
+      <c r="AD4" s="93">
         <f>AD5</f>
         <v>44823</v>
       </c>
-      <c r="AE4" s="96"/>
-      <c r="AF4" s="96"/>
-      <c r="AG4" s="96"/>
-      <c r="AH4" s="96"/>
-      <c r="AI4" s="96"/>
-      <c r="AJ4" s="97"/>
-      <c r="AK4" s="95">
+      <c r="AE4" s="94"/>
+      <c r="AF4" s="94"/>
+      <c r="AG4" s="94"/>
+      <c r="AH4" s="94"/>
+      <c r="AI4" s="94"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="93">
         <f>AK5</f>
         <v>44830</v>
       </c>
-      <c r="AL4" s="96"/>
-      <c r="AM4" s="96"/>
-      <c r="AN4" s="96"/>
-      <c r="AO4" s="96"/>
-      <c r="AP4" s="96"/>
-      <c r="AQ4" s="97"/>
-      <c r="AR4" s="95">
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="94"/>
+      <c r="AN4" s="94"/>
+      <c r="AO4" s="94"/>
+      <c r="AP4" s="94"/>
+      <c r="AQ4" s="95"/>
+      <c r="AR4" s="93">
         <f>AR5</f>
         <v>44837</v>
       </c>
-      <c r="AS4" s="96"/>
-      <c r="AT4" s="96"/>
-      <c r="AU4" s="96"/>
-      <c r="AV4" s="96"/>
-      <c r="AW4" s="96"/>
-      <c r="AX4" s="97"/>
-      <c r="AY4" s="95">
+      <c r="AS4" s="94"/>
+      <c r="AT4" s="94"/>
+      <c r="AU4" s="94"/>
+      <c r="AV4" s="94"/>
+      <c r="AW4" s="94"/>
+      <c r="AX4" s="95"/>
+      <c r="AY4" s="93">
         <f>AY5</f>
         <v>44844</v>
       </c>
-      <c r="AZ4" s="96"/>
-      <c r="BA4" s="96"/>
-      <c r="BB4" s="96"/>
-      <c r="BC4" s="96"/>
-      <c r="BD4" s="96"/>
-      <c r="BE4" s="97"/>
-      <c r="BF4" s="95">
+      <c r="AZ4" s="94"/>
+      <c r="BA4" s="94"/>
+      <c r="BB4" s="94"/>
+      <c r="BC4" s="94"/>
+      <c r="BD4" s="94"/>
+      <c r="BE4" s="95"/>
+      <c r="BF4" s="93">
         <f>BF5</f>
         <v>44851</v>
       </c>
-      <c r="BG4" s="96"/>
-      <c r="BH4" s="96"/>
-      <c r="BI4" s="96"/>
-      <c r="BJ4" s="96"/>
-      <c r="BK4" s="96"/>
-      <c r="BL4" s="97"/>
-      <c r="BM4" s="95">
+      <c r="BG4" s="94"/>
+      <c r="BH4" s="94"/>
+      <c r="BI4" s="94"/>
+      <c r="BJ4" s="94"/>
+      <c r="BK4" s="94"/>
+      <c r="BL4" s="95"/>
+      <c r="BM4" s="93">
         <f>BM5</f>
         <v>44858</v>
       </c>
-      <c r="BN4" s="96"/>
-      <c r="BO4" s="96"/>
-      <c r="BP4" s="96"/>
-      <c r="BQ4" s="96"/>
-      <c r="BR4" s="96"/>
-      <c r="BS4" s="97"/>
-      <c r="BT4" s="95">
+      <c r="BN4" s="94"/>
+      <c r="BO4" s="94"/>
+      <c r="BP4" s="94"/>
+      <c r="BQ4" s="94"/>
+      <c r="BR4" s="94"/>
+      <c r="BS4" s="95"/>
+      <c r="BT4" s="93">
         <f>BT5</f>
         <v>44865</v>
       </c>
-      <c r="BU4" s="96"/>
-      <c r="BV4" s="96"/>
-      <c r="BW4" s="96"/>
-      <c r="BX4" s="96"/>
-      <c r="BY4" s="96"/>
-      <c r="BZ4" s="97"/>
-      <c r="CA4" s="95">
+      <c r="BU4" s="94"/>
+      <c r="BV4" s="94"/>
+      <c r="BW4" s="94"/>
+      <c r="BX4" s="94"/>
+      <c r="BY4" s="94"/>
+      <c r="BZ4" s="95"/>
+      <c r="CA4" s="93">
         <f>CA5</f>
         <v>44872</v>
       </c>
-      <c r="CB4" s="96"/>
-      <c r="CC4" s="96"/>
-      <c r="CD4" s="96"/>
-      <c r="CE4" s="96"/>
-      <c r="CF4" s="96"/>
-      <c r="CG4" s="97"/>
-      <c r="CH4" s="95">
+      <c r="CB4" s="94"/>
+      <c r="CC4" s="94"/>
+      <c r="CD4" s="94"/>
+      <c r="CE4" s="94"/>
+      <c r="CF4" s="94"/>
+      <c r="CG4" s="95"/>
+      <c r="CH4" s="93">
         <f>CH5</f>
         <v>44879</v>
       </c>
-      <c r="CI4" s="96"/>
-      <c r="CJ4" s="96"/>
-      <c r="CK4" s="96"/>
-      <c r="CL4" s="96"/>
-      <c r="CM4" s="96"/>
-      <c r="CN4" s="97"/>
-      <c r="CO4" s="95">
+      <c r="CI4" s="94"/>
+      <c r="CJ4" s="94"/>
+      <c r="CK4" s="94"/>
+      <c r="CL4" s="94"/>
+      <c r="CM4" s="94"/>
+      <c r="CN4" s="95"/>
+      <c r="CO4" s="93">
         <f>CO5</f>
         <v>44886</v>
       </c>
-      <c r="CP4" s="96"/>
-      <c r="CQ4" s="96"/>
-      <c r="CR4" s="96"/>
-      <c r="CS4" s="96"/>
-      <c r="CT4" s="96"/>
-      <c r="CU4" s="97"/>
-      <c r="CV4" s="95">
+      <c r="CP4" s="94"/>
+      <c r="CQ4" s="94"/>
+      <c r="CR4" s="94"/>
+      <c r="CS4" s="94"/>
+      <c r="CT4" s="94"/>
+      <c r="CU4" s="95"/>
+      <c r="CV4" s="93">
         <f>CV5</f>
         <v>44893</v>
       </c>
-      <c r="CW4" s="96"/>
-      <c r="CX4" s="96"/>
-      <c r="CY4" s="96"/>
-      <c r="CZ4" s="96"/>
-      <c r="DA4" s="96"/>
-      <c r="DB4" s="97"/>
-      <c r="DC4" s="95">
+      <c r="CW4" s="94"/>
+      <c r="CX4" s="94"/>
+      <c r="CY4" s="94"/>
+      <c r="CZ4" s="94"/>
+      <c r="DA4" s="94"/>
+      <c r="DB4" s="95"/>
+      <c r="DC4" s="93">
         <f>DC5</f>
         <v>44900</v>
       </c>
-      <c r="DD4" s="96"/>
-      <c r="DE4" s="96"/>
-      <c r="DF4" s="96"/>
-      <c r="DG4" s="96"/>
-      <c r="DH4" s="96"/>
-      <c r="DI4" s="97"/>
-      <c r="DJ4" s="95">
+      <c r="DD4" s="94"/>
+      <c r="DE4" s="94"/>
+      <c r="DF4" s="94"/>
+      <c r="DG4" s="94"/>
+      <c r="DH4" s="94"/>
+      <c r="DI4" s="95"/>
+      <c r="DJ4" s="93">
         <f>DJ5</f>
         <v>44907</v>
       </c>
-      <c r="DK4" s="96"/>
-      <c r="DL4" s="96"/>
-      <c r="DM4" s="96"/>
-      <c r="DN4" s="96"/>
-      <c r="DO4" s="96"/>
-      <c r="DP4" s="97"/>
+      <c r="DK4" s="94"/>
+      <c r="DL4" s="94"/>
+      <c r="DM4" s="94"/>
+      <c r="DN4" s="94"/>
+      <c r="DO4" s="94"/>
+      <c r="DP4" s="95"/>
     </row>
     <row r="5" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
@@ -3123,7 +3123,7 @@
         <v>44</v>
       </c>
       <c r="D10" s="88">
-        <v>0.1111111111111111</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="E10" s="63">
         <f>E9</f>
@@ -5516,6 +5516,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="DJ4:DP4"/>
@@ -5524,17 +5535,6 @@
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <conditionalFormatting sqref="D7:D12 D14:D28">

</xml_diff>

<commit_message>
Ch 6 & 7 grading
</commit_message>
<xml_diff>
--- a/Class/ECO 266 Work Breakdown.xlsx
+++ b/Class/ECO 266 Work Breakdown.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C2A9C4-D8E3-4491-AB24-6201852ECFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B2A0BA-62D0-44CD-A111-433EF66E0749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2986,7 +2986,7 @@
         <v>43</v>
       </c>
       <c r="D9" s="88">
-        <v>0.33333333333333331</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E9" s="63">
         <v>44816</v>
@@ -3123,7 +3123,7 @@
         <v>44</v>
       </c>
       <c r="D10" s="88">
-        <v>0.22222222222222221</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E10" s="63">
         <f>E9</f>
@@ -3786,8 +3786,8 @@
         <v>46</v>
       </c>
       <c r="D15" s="92">
-        <f>6/18</f>
-        <v>0.33333333333333331</v>
+        <f>18/18</f>
+        <v>1</v>
       </c>
       <c r="E15" s="64">
         <v>44819</v>

</xml_diff>

<commit_message>
chapter 8 and test 2
</commit_message>
<xml_diff>
--- a/Class/ECO 266 Work Breakdown.xlsx
+++ b/Class/ECO 266 Work Breakdown.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B2A0BA-62D0-44CD-A111-433EF66E0749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C6D3B2-E8AB-4188-90EE-EEACF24973B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>Task 3</t>
   </si>
@@ -937,23 +937,23 @@
     <xf numFmtId="12" fontId="5" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1620,8 +1620,8 @@
   <dimension ref="A1:DP31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1667,186 +1667,186 @@
         <v>39</v>
       </c>
       <c r="B3" s="62"/>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="98">
+      <c r="D3" s="98"/>
+      <c r="E3" s="96">
         <v>44802</v>
       </c>
-      <c r="F3" s="98"/>
+      <c r="F3" s="96"/>
     </row>
     <row r="4" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="94"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="95">
+      <c r="I4" s="93">
         <f>I5</f>
         <v>44802</v>
       </c>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="95">
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="93">
         <f>P5</f>
         <v>44809</v>
       </c>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="96"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="96"/>
-      <c r="U4" s="96"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="95">
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
+      <c r="S4" s="94"/>
+      <c r="T4" s="94"/>
+      <c r="U4" s="94"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="93">
         <f>W5</f>
         <v>44816</v>
       </c>
-      <c r="X4" s="96"/>
-      <c r="Y4" s="96"/>
-      <c r="Z4" s="96"/>
-      <c r="AA4" s="96"/>
-      <c r="AB4" s="96"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="95">
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="95"/>
+      <c r="AD4" s="93">
         <f>AD5</f>
         <v>44823</v>
       </c>
-      <c r="AE4" s="96"/>
-      <c r="AF4" s="96"/>
-      <c r="AG4" s="96"/>
-      <c r="AH4" s="96"/>
-      <c r="AI4" s="96"/>
-      <c r="AJ4" s="97"/>
-      <c r="AK4" s="95">
+      <c r="AE4" s="94"/>
+      <c r="AF4" s="94"/>
+      <c r="AG4" s="94"/>
+      <c r="AH4" s="94"/>
+      <c r="AI4" s="94"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="93">
         <f>AK5</f>
         <v>44830</v>
       </c>
-      <c r="AL4" s="96"/>
-      <c r="AM4" s="96"/>
-      <c r="AN4" s="96"/>
-      <c r="AO4" s="96"/>
-      <c r="AP4" s="96"/>
-      <c r="AQ4" s="97"/>
-      <c r="AR4" s="95">
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="94"/>
+      <c r="AN4" s="94"/>
+      <c r="AO4" s="94"/>
+      <c r="AP4" s="94"/>
+      <c r="AQ4" s="95"/>
+      <c r="AR4" s="93">
         <f>AR5</f>
         <v>44837</v>
       </c>
-      <c r="AS4" s="96"/>
-      <c r="AT4" s="96"/>
-      <c r="AU4" s="96"/>
-      <c r="AV4" s="96"/>
-      <c r="AW4" s="96"/>
-      <c r="AX4" s="97"/>
-      <c r="AY4" s="95">
+      <c r="AS4" s="94"/>
+      <c r="AT4" s="94"/>
+      <c r="AU4" s="94"/>
+      <c r="AV4" s="94"/>
+      <c r="AW4" s="94"/>
+      <c r="AX4" s="95"/>
+      <c r="AY4" s="93">
         <f>AY5</f>
         <v>44844</v>
       </c>
-      <c r="AZ4" s="96"/>
-      <c r="BA4" s="96"/>
-      <c r="BB4" s="96"/>
-      <c r="BC4" s="96"/>
-      <c r="BD4" s="96"/>
-      <c r="BE4" s="97"/>
-      <c r="BF4" s="95">
+      <c r="AZ4" s="94"/>
+      <c r="BA4" s="94"/>
+      <c r="BB4" s="94"/>
+      <c r="BC4" s="94"/>
+      <c r="BD4" s="94"/>
+      <c r="BE4" s="95"/>
+      <c r="BF4" s="93">
         <f>BF5</f>
         <v>44851</v>
       </c>
-      <c r="BG4" s="96"/>
-      <c r="BH4" s="96"/>
-      <c r="BI4" s="96"/>
-      <c r="BJ4" s="96"/>
-      <c r="BK4" s="96"/>
-      <c r="BL4" s="97"/>
-      <c r="BM4" s="95">
+      <c r="BG4" s="94"/>
+      <c r="BH4" s="94"/>
+      <c r="BI4" s="94"/>
+      <c r="BJ4" s="94"/>
+      <c r="BK4" s="94"/>
+      <c r="BL4" s="95"/>
+      <c r="BM4" s="93">
         <f>BM5</f>
         <v>44858</v>
       </c>
-      <c r="BN4" s="96"/>
-      <c r="BO4" s="96"/>
-      <c r="BP4" s="96"/>
-      <c r="BQ4" s="96"/>
-      <c r="BR4" s="96"/>
-      <c r="BS4" s="97"/>
-      <c r="BT4" s="95">
+      <c r="BN4" s="94"/>
+      <c r="BO4" s="94"/>
+      <c r="BP4" s="94"/>
+      <c r="BQ4" s="94"/>
+      <c r="BR4" s="94"/>
+      <c r="BS4" s="95"/>
+      <c r="BT4" s="93">
         <f>BT5</f>
         <v>44865</v>
       </c>
-      <c r="BU4" s="96"/>
-      <c r="BV4" s="96"/>
-      <c r="BW4" s="96"/>
-      <c r="BX4" s="96"/>
-      <c r="BY4" s="96"/>
-      <c r="BZ4" s="97"/>
-      <c r="CA4" s="95">
+      <c r="BU4" s="94"/>
+      <c r="BV4" s="94"/>
+      <c r="BW4" s="94"/>
+      <c r="BX4" s="94"/>
+      <c r="BY4" s="94"/>
+      <c r="BZ4" s="95"/>
+      <c r="CA4" s="93">
         <f>CA5</f>
         <v>44872</v>
       </c>
-      <c r="CB4" s="96"/>
-      <c r="CC4" s="96"/>
-      <c r="CD4" s="96"/>
-      <c r="CE4" s="96"/>
-      <c r="CF4" s="96"/>
-      <c r="CG4" s="97"/>
-      <c r="CH4" s="95">
+      <c r="CB4" s="94"/>
+      <c r="CC4" s="94"/>
+      <c r="CD4" s="94"/>
+      <c r="CE4" s="94"/>
+      <c r="CF4" s="94"/>
+      <c r="CG4" s="95"/>
+      <c r="CH4" s="93">
         <f>CH5</f>
         <v>44879</v>
       </c>
-      <c r="CI4" s="96"/>
-      <c r="CJ4" s="96"/>
-      <c r="CK4" s="96"/>
-      <c r="CL4" s="96"/>
-      <c r="CM4" s="96"/>
-      <c r="CN4" s="97"/>
-      <c r="CO4" s="95">
+      <c r="CI4" s="94"/>
+      <c r="CJ4" s="94"/>
+      <c r="CK4" s="94"/>
+      <c r="CL4" s="94"/>
+      <c r="CM4" s="94"/>
+      <c r="CN4" s="95"/>
+      <c r="CO4" s="93">
         <f>CO5</f>
         <v>44886</v>
       </c>
-      <c r="CP4" s="96"/>
-      <c r="CQ4" s="96"/>
-      <c r="CR4" s="96"/>
-      <c r="CS4" s="96"/>
-      <c r="CT4" s="96"/>
-      <c r="CU4" s="97"/>
-      <c r="CV4" s="95">
+      <c r="CP4" s="94"/>
+      <c r="CQ4" s="94"/>
+      <c r="CR4" s="94"/>
+      <c r="CS4" s="94"/>
+      <c r="CT4" s="94"/>
+      <c r="CU4" s="95"/>
+      <c r="CV4" s="93">
         <f>CV5</f>
         <v>44893</v>
       </c>
-      <c r="CW4" s="96"/>
-      <c r="CX4" s="96"/>
-      <c r="CY4" s="96"/>
-      <c r="CZ4" s="96"/>
-      <c r="DA4" s="96"/>
-      <c r="DB4" s="97"/>
-      <c r="DC4" s="95">
+      <c r="CW4" s="94"/>
+      <c r="CX4" s="94"/>
+      <c r="CY4" s="94"/>
+      <c r="CZ4" s="94"/>
+      <c r="DA4" s="94"/>
+      <c r="DB4" s="95"/>
+      <c r="DC4" s="93">
         <f>DC5</f>
         <v>44900</v>
       </c>
-      <c r="DD4" s="96"/>
-      <c r="DE4" s="96"/>
-      <c r="DF4" s="96"/>
-      <c r="DG4" s="96"/>
-      <c r="DH4" s="96"/>
-      <c r="DI4" s="97"/>
-      <c r="DJ4" s="95">
+      <c r="DD4" s="94"/>
+      <c r="DE4" s="94"/>
+      <c r="DF4" s="94"/>
+      <c r="DG4" s="94"/>
+      <c r="DH4" s="94"/>
+      <c r="DI4" s="95"/>
+      <c r="DJ4" s="93">
         <f>DJ5</f>
         <v>44907</v>
       </c>
-      <c r="DK4" s="96"/>
-      <c r="DL4" s="96"/>
-      <c r="DM4" s="96"/>
-      <c r="DN4" s="96"/>
-      <c r="DO4" s="96"/>
-      <c r="DP4" s="97"/>
+      <c r="DK4" s="94"/>
+      <c r="DL4" s="94"/>
+      <c r="DM4" s="94"/>
+      <c r="DN4" s="94"/>
+      <c r="DO4" s="94"/>
+      <c r="DP4" s="95"/>
     </row>
     <row r="5" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
@@ -2986,7 +2986,7 @@
         <v>43</v>
       </c>
       <c r="D9" s="88">
-        <v>0.44444444444444442</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="E9" s="63">
         <v>44816</v>
@@ -3123,7 +3123,7 @@
         <v>44</v>
       </c>
       <c r="D10" s="88">
-        <v>0.33333333333333331</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="E10" s="63">
         <f>E9</f>
@@ -3391,8 +3391,8 @@
       <c r="C12" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="88" t="s">
-        <v>45</v>
+      <c r="D12" s="88">
+        <v>1</v>
       </c>
       <c r="E12" s="63">
         <v>44823</v>
@@ -5516,6 +5516,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="DJ4:DP4"/>
@@ -5524,17 +5535,6 @@
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <conditionalFormatting sqref="D7:D12 D14:D28">

</xml_diff>